<commit_message>
Updated values for enemies, towers and bullets
These are more accurate to the balanced, final values they will have.
Will definitely need some testing to finalise.
</commit_message>
<xml_diff>
--- a/docs/tower_enemy_plans.xlsx
+++ b/docs/tower_enemy_plans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edhoc\Documents\Programming\td_game\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C4423E-E81F-4B84-9184-CBA44D7DD740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D145D9-9999-4679-8415-B954139D3F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15480" xr2:uid="{9A0F9C71-3233-439C-8767-21219972ECCD}"/>
+    <workbookView xWindow="1380" yWindow="1380" windowWidth="26055" windowHeight="13455" xr2:uid="{9A0F9C71-3233-439C-8767-21219972ECCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -571,12 +571,16 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T16" sqref="P16:T27"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +624,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -668,7 +672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -716,7 +720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -764,7 +768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -812,7 +816,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -860,7 +864,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -908,7 +912,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -956,7 +960,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1004,7 +1008,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1028,7 +1032,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1052,7 +1056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1076,7 +1080,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1100,7 +1104,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1124,7 +1128,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1148,7 +1152,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1172,7 +1176,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1196,7 +1200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1220,7 +1224,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1244,7 +1248,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1268,7 +1272,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1292,7 +1296,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1316,7 +1320,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1340,7 +1344,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1364,7 +1368,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1388,7 +1392,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1412,7 +1416,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Added script to evaluate difficulty of rounds for balance
This determines how difficult a round will roughly be in terms of the
emeies that are created. It is modelled as a flow of enemies, and
reports both the damage per secomd coming through, and the damage
persecond over a 10 second period. 10s was chosen arbitrarily, but it
felt like enemis would not spend more than 10s in the range of a tower.
As such any more enemies woulld not massively add to the difficulty,
since if it could clear al those in teh 10 period, it could clear any
number of enemies. Likewise if it could not clear them, it would be a
hard round.

Also included the percentage increases of difficulty for each metric.
This shows if the rounds increase in a consisteny manner.

In general, it's quite rough and certainly could be refined. But I think
along side some simulations and play testing, it should hopefully prove
useful.
</commit_message>
<xml_diff>
--- a/docs/tower_enemy_plans.xlsx
+++ b/docs/tower_enemy_plans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edhoc\Documents\Programming\td_game\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D145D9-9999-4679-8415-B954139D3F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611E91C7-DAAF-4242-90E1-6C1AD1E09C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1380" windowWidth="26055" windowHeight="13455" xr2:uid="{9A0F9C71-3233-439C-8767-21219972ECCD}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{9A0F9C71-3233-439C-8767-21219972ECCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -571,7 +571,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,11 +852,11 @@
         <v>0.17</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="1"/>
+        <f>(D6*E6*G6*H6*I6)/J6</f>
         <v>0.17</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(K6,L6)</f>
         <v>0.17</v>
       </c>
       <c r="N6">
@@ -908,7 +908,7 @@
         <v>0.1875</v>
       </c>
       <c r="N7">
-        <f t="shared" si="3"/>
+        <f>E7*H7</f>
         <v>30</v>
       </c>
     </row>
@@ -956,7 +956,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="N8">
-        <f t="shared" si="3"/>
+        <f>E8*H8</f>
         <v>360</v>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="N9">
-        <f t="shared" si="3"/>
+        <f>E9*H9</f>
         <v>200</v>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
         <v>42</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C25">
         <v>0.9</v>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="G25">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1325,7 +1325,7 @@
         <v>47</v>
       </c>
       <c r="B26">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C26">
         <v>0.8</v>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="G26">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added the rest of the slime enemies
This was four more, medium, large, giant and uber. Each one had the same
animation, but a different size and colour.

ALso had to make some changes to the game config and bullet mechanics.
Because the slimes are slow, the rounding down of enemy steps meant the
larger and slower slimes had 0 speed. To resolve this, the subgrid size
was increased. This seems to not have affected performance. It did
however slow down all the bullets, as their speed was a fixed value.
This has been changed so that the speed is independent of the subgrid
size.
</commit_message>
<xml_diff>
--- a/docs/tower_enemy_plans.xlsx
+++ b/docs/tower_enemy_plans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edhoc\Documents\Programming\td_game\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611E91C7-DAAF-4242-90E1-6C1AD1E09C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AF9CB6-F176-43A6-8B26-2EF4A57C379D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{9A0F9C71-3233-439C-8767-21219972ECCD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A0F9C71-3233-439C-8767-21219972ECCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -571,7 +571,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added new enemy types
These are two more bonehead types. The shield one has resistances, which
is a new property of enemys that has also been added in this comit.
Resistance halves damage from a given bullet type. Some enemies have had
weaknesses added. Weakness doubles damage from certain bullet types.

The bonelord is a very large and strong enemy.
</commit_message>
<xml_diff>
--- a/docs/tower_enemy_plans.xlsx
+++ b/docs/tower_enemy_plans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edhoc\Documents\Programming\td_game\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AF9CB6-F176-43A6-8B26-2EF4A57C379D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4397F049-0B36-444C-A511-DF751691FB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A0F9C71-3233-439C-8767-21219972ECCD}"/>
+    <workbookView xWindow="1410" yWindow="1395" windowWidth="26040" windowHeight="13440" xr2:uid="{9A0F9C71-3233-439C-8767-21219972ECCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>Tower</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>HPps</t>
+  </si>
+  <si>
+    <t>Fire, rock</t>
   </si>
 </sst>
 </file>
@@ -571,7 +574,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,7 +719,7 @@
         <v>0.16</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N9" si="3">E3*H3</f>
+        <f t="shared" ref="N3:N6" si="3">E3*H3</f>
         <v>4</v>
       </c>
     </row>
@@ -1067,7 +1070,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
         <v>31</v>

</xml_diff>